<commit_message>
Added readme update with more detials and information on the intake instructions file that was added. also corrected some issues in the intake file that were note saved somehow
</commit_message>
<xml_diff>
--- a/production_system_intake_Example01.xlsx
+++ b/production_system_intake_Example01.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Classes\2025_01_Spring\ASU\Computation\Week03\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Classes\2025_01_Spring\ASU\Computation\Week03\Project\Dev\CAS502Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AA392E-98D5-4F16-9DE3-8D1522FA21D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914D405A-E54E-4632-BCDE-5ECA0DEBE0F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2130" windowWidth="29040" windowHeight="15840" tabRatio="857" firstSheet="9" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="570" yWindow="4680" windowWidth="37830" windowHeight="15435" tabRatio="857" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProcessorTypeTbl" sheetId="3" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1538" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1509" uniqueCount="589">
   <si>
     <t>TaskIndex</t>
   </si>
@@ -4713,7 +4713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22DCE508-4EF3-4CE2-915A-C48C27323B08}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
@@ -13502,10 +13502,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E098E04-19A8-4E79-81CD-069FB2C95590}">
-  <dimension ref="A1:BA82"/>
+  <dimension ref="A1:BA81"/>
   <sheetViews>
-    <sheetView topLeftCell="N16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE24" sqref="AE24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13535,278 +13535,212 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="D1" t="s">
-        <v>344</v>
-      </c>
-      <c r="E1" t="s">
-        <v>345</v>
-      </c>
-      <c r="F1" t="s">
-        <v>141</v>
-      </c>
-      <c r="G1" t="s">
-        <v>346</v>
-      </c>
-      <c r="H1" t="s">
-        <v>144</v>
-      </c>
-      <c r="I1" t="s">
-        <v>146</v>
-      </c>
-      <c r="J1" t="s">
-        <v>149</v>
-      </c>
-      <c r="K1" t="s">
-        <v>152</v>
-      </c>
-      <c r="L1" t="s">
-        <v>154</v>
-      </c>
-      <c r="M1" t="s">
-        <v>156</v>
-      </c>
-      <c r="N1" t="s">
-        <v>158</v>
-      </c>
-      <c r="O1" t="s">
-        <v>160</v>
-      </c>
-      <c r="P1" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>164</v>
-      </c>
-      <c r="R1" t="s">
-        <v>355</v>
-      </c>
-      <c r="S1" t="s">
-        <v>168</v>
-      </c>
-      <c r="T1" t="s">
-        <v>347</v>
-      </c>
-      <c r="U1" t="s">
-        <v>171</v>
-      </c>
-      <c r="V1" t="s">
-        <v>348</v>
-      </c>
-      <c r="W1" t="s">
-        <v>349</v>
-      </c>
-      <c r="X1" t="s">
-        <v>350</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>351</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>177</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>352</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>353</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>354</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>182</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>184</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>356</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="AI2" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="AJ2" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="AL2" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="AM2" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="AN2" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="AO2" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="AP2" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="AQ2" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="AR2" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="AS2" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="AT2" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="AU2" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="AV2" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="AW2" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="AX2" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="AY2" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="AZ2" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="BA2" s="1" t="s">
-        <v>430</v>
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>325</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>325</v>
+        <v>20</v>
       </c>
       <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="AE3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>331</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -13817,21 +13751,22 @@
       <c r="J4">
         <v>1</v>
       </c>
-      <c r="AE4">
+      <c r="Q4">
+        <f>SUM(D4:G4)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>331</v>
-      </c>
-      <c r="E5">
+        <v>326</v>
+      </c>
+      <c r="D5">
         <v>1</v>
       </c>
       <c r="I5">
@@ -13841,19 +13776,19 @@
         <v>1</v>
       </c>
       <c r="Q5">
-        <f>SUM(D5:G5)</f>
+        <f t="shared" ref="Q5:Q68" si="0">SUM(D5:G5)</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -13865,19 +13800,19 @@
         <v>1</v>
       </c>
       <c r="Q6">
-        <f t="shared" ref="Q6:Q69" si="0">SUM(D6:G6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -13895,13 +13830,13 @@
     </row>
     <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -13919,15 +13854,15 @@
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>329</v>
-      </c>
-      <c r="D9">
+        <v>330</v>
+      </c>
+      <c r="E9">
         <v>1</v>
       </c>
       <c r="I9">
@@ -13943,15 +13878,18 @@
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>330</v>
+        <v>359</v>
       </c>
       <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
         <v>1</v>
       </c>
       <c r="I10">
@@ -13962,23 +13900,23 @@
       </c>
       <c r="Q10">
         <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="R10">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>359</v>
+        <v>334</v>
       </c>
       <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
         <v>1</v>
       </c>
       <c r="I11">
@@ -13989,21 +13927,21 @@
       </c>
       <c r="Q11">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="R11">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>334</v>
+        <v>32</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -14016,21 +13954,21 @@
       </c>
       <c r="Q12">
         <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="X12">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
+        <v>332</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -14043,23 +13981,23 @@
       </c>
       <c r="Q13">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="X13">
+        <v>1</v>
+      </c>
+      <c r="AE13">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>332</v>
-      </c>
-      <c r="E14">
+        <v>336</v>
+      </c>
+      <c r="D14">
         <v>1</v>
       </c>
       <c r="I14">
@@ -14072,19 +14010,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AE14">
-        <v>1</v>
-      </c>
     </row>
     <row r="15" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -14102,13 +14037,13 @@
     </row>
     <row r="16" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -14126,15 +14061,18 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="G17">
         <v>1</v>
       </c>
       <c r="I17">
@@ -14145,23 +14083,23 @@
       </c>
       <c r="Q17">
         <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="T17">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="G18">
         <v>1</v>
       </c>
       <c r="I18">
@@ -14172,21 +14110,18 @@
       </c>
       <c r="Q18">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="T18">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -14201,16 +14136,22 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="W19">
+        <v>1</v>
+      </c>
+      <c r="AC19">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -14225,22 +14166,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="W20">
-        <v>1</v>
-      </c>
-      <c r="AC20">
-        <v>1</v>
-      </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -14258,15 +14193,15 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>343</v>
-      </c>
-      <c r="D22">
+        <v>357</v>
+      </c>
+      <c r="E22">
         <v>1</v>
       </c>
       <c r="I22">
@@ -14282,15 +14217,18 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
         <v>1</v>
       </c>
       <c r="I23">
@@ -14301,23 +14239,23 @@
       </c>
       <c r="Q23">
         <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="Y23">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
       <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24">
         <v>1</v>
       </c>
       <c r="I24">
@@ -14328,21 +14266,24 @@
       </c>
       <c r="Q24">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="Y24">
+        <v>1</v>
+      </c>
+      <c r="R24">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>363</v>
+        <v>48</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -14355,24 +14296,18 @@
       </c>
       <c r="Q25">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R25">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
+        <v>362</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -14385,18 +14320,21 @@
       </c>
       <c r="Q26">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="AE26">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>362</v>
+        <v>53</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -14411,21 +14349,18 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AE27">
-        <v>1</v>
-      </c>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28">
+        <v>364</v>
+      </c>
+      <c r="D28">
         <v>1</v>
       </c>
       <c r="I28">
@@ -14441,13 +14376,13 @@
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" t="s">
-        <v>364</v>
+        <v>55</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>365</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -14465,13 +14400,13 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>365</v>
+        <v>56</v>
+      </c>
+      <c r="C30" t="s">
+        <v>366</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -14489,13 +14424,13 @@
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C31" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -14513,15 +14448,18 @@
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C32" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
         <v>1</v>
       </c>
       <c r="I32">
@@ -14532,21 +14470,21 @@
       </c>
       <c r="Q32">
         <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AA32">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C33" t="s">
-        <v>368</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
+        <v>369</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -14559,23 +14497,23 @@
       </c>
       <c r="Q33">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="AA33">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C34" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
         <v>1</v>
       </c>
       <c r="I34">
@@ -14586,23 +14524,20 @@
       </c>
       <c r="Q34">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C35" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="E35">
-        <v>1</v>
-      </c>
-      <c r="F35">
         <v>1</v>
       </c>
       <c r="I35">
@@ -14613,18 +14548,24 @@
       </c>
       <c r="Q35">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="W35">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C36" t="s">
-        <v>370</v>
+        <v>63</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -14637,24 +14578,18 @@
       </c>
       <c r="Q36">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="W36">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C37" t="s">
-        <v>63</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
+        <v>333</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -14667,20 +14602,23 @@
       </c>
       <c r="Q37">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="AE37">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C38" t="s">
-        <v>333</v>
-      </c>
-      <c r="E38">
+        <v>371</v>
+      </c>
+      <c r="D38">
         <v>1</v>
       </c>
       <c r="I38">
@@ -14693,19 +14631,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AE38">
-        <v>1</v>
-      </c>
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C39" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -14723,13 +14658,13 @@
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C40" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -14744,18 +14679,24 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="R40">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C41" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="G41">
         <v>1</v>
       </c>
       <c r="I41">
@@ -14766,26 +14707,20 @@
       </c>
       <c r="Q41">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R41">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C42" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D42">
-        <v>1</v>
-      </c>
-      <c r="G42">
         <v>1</v>
       </c>
       <c r="I42">
@@ -14796,18 +14731,18 @@
       </c>
       <c r="Q42">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C43" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -14825,13 +14760,13 @@
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C44" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -14849,15 +14784,15 @@
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C45" t="s">
-        <v>377</v>
-      </c>
-      <c r="D45">
+        <v>378</v>
+      </c>
+      <c r="E45">
         <v>1</v>
       </c>
       <c r="I45">
@@ -14870,18 +14805,21 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="V45">
+        <v>1</v>
+      </c>
     </row>
     <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C46" t="s">
-        <v>378</v>
-      </c>
-      <c r="E46">
+        <v>379</v>
+      </c>
+      <c r="D46">
         <v>1</v>
       </c>
       <c r="I46">
@@ -14894,21 +14832,18 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="V46">
-        <v>1</v>
-      </c>
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C47" t="s">
-        <v>379</v>
-      </c>
-      <c r="D47">
+        <v>380</v>
+      </c>
+      <c r="E47">
         <v>1</v>
       </c>
       <c r="I47">
@@ -14921,18 +14856,24 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="T47">
+        <v>1</v>
+      </c>
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C48" t="s">
-        <v>380</v>
+        <v>361</v>
       </c>
       <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
         <v>1</v>
       </c>
       <c r="I48">
@@ -14943,26 +14884,20 @@
       </c>
       <c r="Q48">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="T48">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C49" t="s">
-        <v>361</v>
+        <v>335</v>
       </c>
       <c r="E49">
-        <v>1</v>
-      </c>
-      <c r="F49">
         <v>1</v>
       </c>
       <c r="I49">
@@ -14973,18 +14908,21 @@
       </c>
       <c r="Q49">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C50" t="s">
-        <v>335</v>
+        <v>80</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -14997,21 +14935,21 @@
       </c>
       <c r="Q50">
         <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AB50">
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C51" t="s">
-        <v>80</v>
-      </c>
-      <c r="D51">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="E51">
         <v>1</v>
@@ -15024,21 +14962,21 @@
       </c>
       <c r="Q51">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="AB51">
+        <v>1</v>
+      </c>
+      <c r="AE51">
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C52" t="s">
-        <v>82</v>
+        <v>431</v>
       </c>
       <c r="E52">
         <v>1</v>
@@ -15053,19 +14991,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AE52">
-        <v>1</v>
-      </c>
     </row>
     <row r="53" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C53" t="s">
-        <v>431</v>
+        <v>87</v>
       </c>
       <c r="E53">
         <v>1</v>
@@ -15080,18 +15015,24 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="S53">
+        <v>1</v>
+      </c>
+      <c r="U53">
+        <v>1</v>
+      </c>
     </row>
     <row r="54" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C54" t="s">
-        <v>87</v>
-      </c>
-      <c r="E54">
+        <v>432</v>
+      </c>
+      <c r="D54">
         <v>1</v>
       </c>
       <c r="I54">
@@ -15104,22 +15045,19 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="S54">
-        <v>1</v>
-      </c>
-      <c r="U54">
+      <c r="AC54">
         <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C55" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -15134,19 +15072,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AC55">
-        <v>1</v>
-      </c>
     </row>
     <row r="56" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C56" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -15164,15 +15099,18 @@
     </row>
     <row r="57" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C57" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="G57">
         <v>1</v>
       </c>
       <c r="I57">
@@ -15183,23 +15121,20 @@
       </c>
       <c r="Q57">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C58" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D58">
-        <v>1</v>
-      </c>
-      <c r="G58">
         <v>1</v>
       </c>
       <c r="I58">
@@ -15210,20 +15145,20 @@
       </c>
       <c r="Q58">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C59" t="s">
-        <v>436</v>
-      </c>
-      <c r="D59">
+        <v>94</v>
+      </c>
+      <c r="E59">
         <v>1</v>
       </c>
       <c r="I59">
@@ -15239,15 +15174,15 @@
     </row>
     <row r="60" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C60" t="s">
-        <v>94</v>
-      </c>
-      <c r="E60">
+        <v>437</v>
+      </c>
+      <c r="D60">
         <v>1</v>
       </c>
       <c r="I60">
@@ -15260,18 +15195,24 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="Z60">
+        <v>1</v>
+      </c>
     </row>
     <row r="61" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C61" t="s">
-        <v>437</v>
-      </c>
-      <c r="D61">
+        <v>439</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61">
         <v>1</v>
       </c>
       <c r="I61">
@@ -15282,26 +15223,20 @@
       </c>
       <c r="Q61">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="Z61">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C62" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="E62">
-        <v>1</v>
-      </c>
-      <c r="F62">
         <v>1</v>
       </c>
       <c r="I62">
@@ -15312,18 +15247,21 @@
       </c>
       <c r="Q62">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C63" t="s">
-        <v>440</v>
+        <v>99</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
       </c>
       <c r="E63">
         <v>1</v>
@@ -15336,21 +15274,18 @@
       </c>
       <c r="Q63">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C64" t="s">
-        <v>99</v>
-      </c>
-      <c r="D64">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="E64">
         <v>1</v>
@@ -15363,18 +15298,21 @@
       </c>
       <c r="Q64">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="AE64">
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C65" t="s">
-        <v>101</v>
+        <v>441</v>
       </c>
       <c r="E65">
         <v>1</v>
@@ -15389,19 +15327,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AE65">
-        <v>1</v>
-      </c>
     </row>
     <row r="66" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C66" t="s">
-        <v>441</v>
+        <v>106</v>
       </c>
       <c r="E66">
         <v>1</v>
@@ -15419,15 +15354,15 @@
     </row>
     <row r="67" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C67" t="s">
-        <v>106</v>
-      </c>
-      <c r="E67">
+        <v>442</v>
+      </c>
+      <c r="D67">
         <v>1</v>
       </c>
       <c r="I67">
@@ -15443,13 +15378,13 @@
     </row>
     <row r="68" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C68" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -15467,15 +15402,15 @@
     </row>
     <row r="69" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C69" t="s">
-        <v>444</v>
-      </c>
-      <c r="D69">
+        <v>443</v>
+      </c>
+      <c r="E69">
         <v>1</v>
       </c>
       <c r="I69">
@@ -15485,23 +15420,29 @@
         <v>1</v>
       </c>
       <c r="Q69">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Q69:Q70" si="1">SUM(D69:G69)</f>
         <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C70" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="E70">
         <v>1</v>
       </c>
+      <c r="F70">
+        <v>1</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
       <c r="I70">
         <v>1</v>
       </c>
@@ -15509,49 +15450,42 @@
         <v>1</v>
       </c>
       <c r="Q70">
-        <f t="shared" ref="Q70:Q71" si="1">SUM(D70:G70)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C71" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E71">
         <v>1</v>
       </c>
-      <c r="F71">
-        <v>1</v>
-      </c>
-      <c r="G71">
-        <v>1</v>
-      </c>
       <c r="I71">
         <v>1</v>
       </c>
       <c r="J71">
         <v>1</v>
-      </c>
-      <c r="Q71">
-        <f t="shared" si="1"/>
-        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C72" t="s">
-        <v>445</v>
+        <v>113</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -15565,62 +15499,59 @@
     </row>
     <row r="73" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C73" t="s">
-        <v>113</v>
-      </c>
-      <c r="D73">
-        <v>1</v>
+        <v>457</v>
       </c>
       <c r="E73">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I73">
         <v>1</v>
       </c>
-      <c r="J73">
+      <c r="AF73">
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C74" t="s">
-        <v>457</v>
+        <v>453</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
       </c>
       <c r="E74">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I74">
-        <v>1</v>
-      </c>
-      <c r="AF74">
         <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C75" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D75">
         <v>1</v>
       </c>
       <c r="E75">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I75">
         <v>1</v>
@@ -15628,53 +15559,59 @@
     </row>
     <row r="76" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C76" t="s">
-        <v>455</v>
-      </c>
-      <c r="D76">
-        <v>1</v>
-      </c>
-      <c r="E76">
-        <v>4</v>
+        <v>456</v>
       </c>
       <c r="I76">
+        <v>1</v>
+      </c>
+      <c r="N76">
+        <v>1</v>
+      </c>
+      <c r="P76">
         <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C77" t="s">
-        <v>456</v>
+        <v>462</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+      <c r="F77">
+        <v>1</v>
       </c>
       <c r="I77">
         <v>1</v>
       </c>
-      <c r="N77">
-        <v>1</v>
-      </c>
-      <c r="P77">
+      <c r="O77">
         <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C78" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D78">
         <v>1</v>
@@ -15686,92 +15623,66 @@
         <v>1</v>
       </c>
       <c r="I78">
-        <v>1</v>
-      </c>
-      <c r="O78">
         <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C79" t="s">
-        <v>460</v>
-      </c>
-      <c r="D79">
-        <v>1</v>
+        <v>458</v>
       </c>
       <c r="E79">
-        <v>1</v>
-      </c>
-      <c r="F79">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="H79">
+        <v>2</v>
       </c>
       <c r="I79">
+        <v>1</v>
+      </c>
+      <c r="L79">
+        <v>1</v>
+      </c>
+      <c r="M79">
         <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C80" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="E80">
         <v>3</v>
       </c>
       <c r="H80">
-        <v>2</v>
-      </c>
-      <c r="I80">
-        <v>1</v>
-      </c>
-      <c r="L80">
+        <v>1</v>
+      </c>
+      <c r="K80">
         <v>1</v>
       </c>
       <c r="M80">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C81" t="s">
-        <v>459</v>
-      </c>
-      <c r="E81">
-        <v>3</v>
-      </c>
-      <c r="H81">
-        <v>1</v>
-      </c>
-      <c r="K81">
-        <v>1</v>
-      </c>
-      <c r="M81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>79</v>
-      </c>
-      <c r="B82" t="s">
-        <v>123</v>
-      </c>
-      <c r="C82" t="s">
         <v>452</v>
       </c>
     </row>

</xml_diff>